<commit_message>
13 rename several classes, add quick swap function , add handler of buttons in grid pane, add randSortM, fix some bugs, modify init process, add GlobalVariables
</commit_message>
<xml_diff>
--- a/src/cn/rocket/deksrt/resource/templateOfStuInfo.xlsx
+++ b/src/cn/rocket/deksrt/resource/templateOfStuInfo.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B459F6F-017E-4BCF-B99A-E04B832880C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="+l4XMoQwIGEcq9le+wIPuOhMZwY0DP9JWWTHvJiOtp9cEt9sXH8v7mgKeu2/4qFI4/TFdGHNIVTyE2JAf6bIZQ==" workbookSaltValue="w9MH/YmBQzxk9OCjOUW1pw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="信息" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -24,22 +26,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>首字母拼音</t>
+    <t>住校填1，否则填0或不填</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>班主任信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否住校项：住校写1，通校留空或0</t>
+    <t>姓名对应拼音(小写)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,7 +62,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -72,13 +70,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -97,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -172,6 +259,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,6 +311,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,50 +503,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F45D66-7C0D-4BC7-BDE6-7FC3E64A8FC7}">
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="//irhLH4Raq3j3cNKU1fZCxLuRLCZUhwtM+39SfQhylwLfnlM9hN3QtepewKrKthMh7iJu92cj4X9iIettpeig==" saltValue="gG8KuCODznGGMHJQDiWanw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="pCDUVK1CiiRLZ/23XjdEFYu+EzQlu8USAqd0bxg1UwSXq9jOiV2knrOKwD1AkKD5lNh5ogqAtMnKG2wOxe5FRQ==" saltValue="GkKaZPqCeh78rQOREl4M7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="B52:C52" name="区域2"/>
-    <protectedRange sqref="A2:C51" name="区域1"/>
+    <protectedRange sqref="A1:C53" name="区域1"/>
   </protectedRanges>
-  <mergeCells count="1">
-    <mergeCell ref="B52:C52"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
21- prepare to release, fix small bugs
</commit_message>
<xml_diff>
--- a/src/cn/rocket/deksrt/resource/templateOfStuInfo.xlsx
+++ b/src/cn/rocket/deksrt/resource/templateOfStuInfo.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B459F6F-017E-4BCF-B99A-E04B832880C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="+l4XMoQwIGEcq9le+wIPuOhMZwY0DP9JWWTHvJiOtp9cEt9sXH8v7mgKeu2/4qFI4/TFdGHNIVTyE2JAf6bIZQ==" workbookSaltValue="w9MH/YmBQzxk9OCjOUW1pw==" workbookSpinCount="100000" lockStructure="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaWorkSpace\DeskSorting\src\cn\rocket\deksrt\resource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A08DA-B825-4136-9B16-24AD40DC30F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="CfL3NK+CwcbpfrXyCcf0AXkPIabJWRw1w6ToROspqwFgYQr/uOpltxm1A+hhK7p5YVgMfes1jyCcyWcyUDHMaQ==" workbookSaltValue="vs0zIony5QzbrFmfEaDJGA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BC9FCFB-41C5-4945-9F1C-D0EF583EBE05}"/>
   </bookViews>
   <sheets>
-    <sheet name="信息" sheetId="2" r:id="rId1"/>
+    <sheet name="学生名单" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -22,15 +32,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>对应拼音（小写，首字母）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>是否住校</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>住校填1，否则填0或不填</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名对应拼音(小写)</t>
+    <t>住校填1，不住校填0或留空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -42,14 +52,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -71,11 +82,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -84,7 +95,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -92,17 +103,17 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
@@ -112,7 +123,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
@@ -120,12 +131,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -134,44 +145,65 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -194,44 +226,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -281,9 +313,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -339,468 +371,439 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F45D66-7C0D-4BC7-BDE6-7FC3E64A8FC7}">
-  <dimension ref="A1:D54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B730C7F-2774-4A4A-BF55-D1577642C515}">
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="7"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pCDUVK1CiiRLZ/23XjdEFYu+EzQlu8USAqd0bxg1UwSXq9jOiV2knrOKwD1AkKD5lNh5ogqAtMnKG2wOxe5FRQ==" saltValue="GkKaZPqCeh78rQOREl4M7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="caApqJCa1iKuELd/DMY6xeyGIVaiy6Q7vpKkkNzJBHGzh5AOWPRoZ3HTa+OpzN3MEekWIa6m3ux1hZew3PezYQ==" saltValue="4HB5qABg40KDoqeHM1hx+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="A1:C53" name="区域1"/>
+    <protectedRange sqref="A2:C53" name="可编辑区域"/>
   </protectedRanges>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>